<commit_message>
service add square method
</commit_message>
<xml_diff>
--- a/CResults.xlsx
+++ b/CResults.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman.chepky\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roman.chepky/IdeaProjects/cwopr/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3317EB83-B000-A147-9D0F-BC2BD728474A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -279,12 +280,21 @@
   </si>
   <si>
     <t>400x267</t>
+  </si>
+  <si>
+    <t>это назвать 1-2</t>
+  </si>
+  <si>
+    <t>остальное нормировать</t>
+  </si>
+  <si>
+    <t>Square</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,14 +369,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -643,21 +654,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,8 +687,11 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -696,8 +710,11 @@
       <c r="F2">
         <v>162139</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>902500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -716,8 +733,11 @@
       <c r="F3">
         <v>125478</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>902500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -736,8 +756,11 @@
       <c r="F4">
         <v>55149</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>902500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -756,8 +779,11 @@
       <c r="F5">
         <v>162778</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1305600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -776,8 +802,11 @@
       <c r="F6">
         <v>52344</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1305600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -796,8 +825,11 @@
       <c r="F7">
         <v>130025</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>1352724</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -816,8 +848,11 @@
       <c r="F8">
         <v>208625</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>23438184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -836,8 +871,11 @@
       <c r="F9">
         <v>27619</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>1352724</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -856,8 +894,11 @@
       <c r="F10">
         <v>149297</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>902500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -876,8 +917,11 @@
       <c r="F11">
         <v>154442</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>902500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -896,8 +940,11 @@
       <c r="F12">
         <v>256</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -916,8 +963,11 @@
       <c r="F13">
         <v>256</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -936,8 +986,11 @@
       <c r="F14">
         <v>134</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -956,8 +1009,11 @@
       <c r="F15">
         <v>256</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -976,8 +1032,11 @@
       <c r="F16">
         <v>236</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -996,8 +1055,11 @@
       <c r="F17">
         <v>255</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1016,8 +1078,11 @@
       <c r="F18">
         <v>447</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1036,8 +1101,11 @@
       <c r="F19">
         <v>465</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1056,8 +1124,11 @@
       <c r="F20">
         <v>384</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1076,8 +1147,11 @@
       <c r="F21">
         <v>386</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1096,8 +1170,11 @@
       <c r="F22">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>240672</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1116,8 +1193,11 @@
       <c r="F23">
         <v>5053</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1136,8 +1216,11 @@
       <c r="F24">
         <v>7810</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>82694</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1156,8 +1239,11 @@
       <c r="F25">
         <v>1357</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1176,8 +1262,11 @@
       <c r="F26">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1196,8 +1285,11 @@
       <c r="F27">
         <v>102</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>50625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1216,8 +1308,11 @@
       <c r="F28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>113564</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1236,8 +1331,11 @@
       <c r="F29">
         <v>2564</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1256,8 +1354,11 @@
       <c r="F30">
         <v>1692</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>112225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1276,8 +1377,11 @@
       <c r="F31">
         <v>6298</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>50530</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1296,8 +1400,11 @@
       <c r="F32">
         <v>263270</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>1749600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1316,8 +1423,11 @@
       <c r="F33">
         <v>229001</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>1350000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1336,8 +1446,11 @@
       <c r="F34">
         <v>170155</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>1066485</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1356,8 +1469,11 @@
       <c r="F35">
         <v>63789</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>699392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1376,8 +1492,11 @@
       <c r="F36">
         <v>125420</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>647000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1396,8 +1515,11 @@
       <c r="F37">
         <v>330514</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>2457600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1416,8 +1538,11 @@
       <c r="F38">
         <v>44746</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>667000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1436,8 +1561,11 @@
       <c r="F39">
         <v>47626</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>667000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1456,8 +1584,11 @@
       <c r="F40">
         <v>112678</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>2056320</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1476,8 +1607,11 @@
       <c r="F41">
         <v>93876</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1496,8 +1630,11 @@
       <c r="F42">
         <v>5868</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1516,8 +1653,11 @@
       <c r="F43">
         <v>20985</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>426756</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1536,8 +1676,11 @@
       <c r="F44">
         <v>10751</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>53190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1556,8 +1699,11 @@
       <c r="F45">
         <v>8656</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>53190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1576,8 +1722,11 @@
       <c r="F46">
         <v>12474</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>53190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1596,8 +1745,11 @@
       <c r="F47">
         <v>11288</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>53190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1616,8 +1768,11 @@
       <c r="F48">
         <v>18394</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>106800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1636,8 +1791,11 @@
       <c r="F49">
         <v>17428</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>106800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1655,6 +1813,19 @@
       </c>
       <c r="F50">
         <v>10993</v>
+      </c>
+      <c r="G50">
+        <v>106800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve excel one more time
</commit_message>
<xml_diff>
--- a/CResults.xlsx
+++ b/CResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>Norm Size</t>
+  </si>
+  <si>
+    <t>Norm Externsion</t>
+  </si>
+  <si>
+    <t>Norm Ratio</t>
+  </si>
+  <si>
+    <t>Norm Color</t>
   </si>
 </sst>
 </file>
@@ -398,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -407,7 +416,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,10 +701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="94" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="94" workbookViewId="0">
+      <selection activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +712,10 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1807,7 +1822,7 @@
         <v>106800</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1830,7 +1845,7 @@
         <v>106800</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1853,18 +1868,18 @@
         <v>106800</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -1883,11 +1898,20 @@
       <c r="F57" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="I57" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J57" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1906,12 +1930,17 @@
       <c r="F58">
         <v>902500</v>
       </c>
+      <c r="I58" s="9">
+        <v>1</v>
+      </c>
       <c r="J58">
-        <f>(C58-MIN(C58:C97))/(MAX(C58:C97) - MIN(C58:C97))</f>
-        <v>7.1887267705853991E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.1887267705853894E-2</v>
+      </c>
+      <c r="K58">
+        <v>0.11565677966101599</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1930,12 +1959,17 @@
       <c r="F59">
         <v>902500</v>
       </c>
+      <c r="I59" s="9">
+        <v>1</v>
+      </c>
       <c r="J59">
-        <f>(C59-MIN(C58:C97))/(MAX(C58:C97) - MIN(C58:C97))</f>
-        <v>5.1849805304544763E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.1849805304544701E-2</v>
+      </c>
+      <c r="K59">
+        <v>0.11565677966101599</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -1954,12 +1988,17 @@
       <c r="F60">
         <v>902500</v>
       </c>
+      <c r="I60" s="9">
+        <v>1</v>
+      </c>
       <c r="J60">
-        <f>(C60-MIN(C58:C97))/(MAX(C58:C97) - MIN(C58:C97))</f>
         <v>7.8397405260296996E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <v>0.11565677966101599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -1978,12 +2017,17 @@
       <c r="F61">
         <v>1305600</v>
       </c>
+      <c r="I61" s="9">
+        <v>1</v>
+      </c>
       <c r="J61">
-        <f>(61-MIN(C58:C97))/(MAX(C58:C97) - MIN(C58:C97))</f>
-        <v>-8.9289447596303719E-4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.128736117660944</v>
+      </c>
+      <c r="K61">
+        <v>0.207265183615819</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2002,12 +2046,17 @@
       <c r="F62">
         <v>1305600</v>
       </c>
+      <c r="I62" s="9">
+        <v>1</v>
+      </c>
       <c r="J62">
-        <f>(C62-MIN(C58:C97))/(MAX(C58:C97) - MIN(C58:C97))</f>
-        <v>5.8880753863343217E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.8880753863343203E-2</v>
+      </c>
+      <c r="K62">
+        <v>0.207265183615819</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -2026,8 +2075,17 @@
       <c r="F63">
         <v>1352724</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I63" s="9">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>0.74796399417580794</v>
+      </c>
+      <c r="K63">
+        <v>0.21254046632033699</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -2046,8 +2104,17 @@
       <c r="F64">
         <v>23438184</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I64" s="9">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>0.72555535972214902</v>
+      </c>
+      <c r="K64">
+        <v>0.21222527189834201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -2066,8 +2133,17 @@
       <c r="F65">
         <v>1352724</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I65" s="9">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>0.113296506067395</v>
+      </c>
+      <c r="K65">
+        <v>0.21254046632033699</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2086,8 +2162,17 @@
       <c r="F66">
         <v>262144</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I66" s="9">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>3.4048548689212901E-3</v>
+      </c>
+      <c r="K66">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -2106,8 +2191,17 @@
       <c r="F67">
         <v>262144</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I67" s="9">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>3.7695284278652899E-3</v>
+      </c>
+      <c r="K67">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -2126,8 +2220,17 @@
       <c r="F68">
         <v>262144</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I68" s="9">
+        <v>0</v>
+      </c>
+      <c r="J68" s="8">
+        <v>2.33941528379171E-4</v>
+      </c>
+      <c r="K68">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2146,8 +2249,17 @@
       <c r="F69">
         <v>262144</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I69" s="9">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>2.6088185370609402E-3</v>
+      </c>
+      <c r="K69">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -2166,8 +2278,17 @@
       <c r="F70">
         <v>262144</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I70" s="9">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>4.6793598470594002E-3</v>
+      </c>
+      <c r="K70">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -2186,8 +2307,17 @@
       <c r="F71">
         <v>262144</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I71" s="9">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>4.50046338418121E-3</v>
+      </c>
+      <c r="K71">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -2206,8 +2336,17 @@
       <c r="F72">
         <v>262144</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I72" s="9">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>5.7410944758571796E-3</v>
+      </c>
+      <c r="K72">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -2226,8 +2365,17 @@
       <c r="F73">
         <v>262144</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I73" s="9">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>8.1408476199095799E-3</v>
+      </c>
+      <c r="K73">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2246,8 +2394,17 @@
       <c r="F74">
         <v>240672</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I74" s="9">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>9.0247443447811198E-3</v>
+      </c>
+      <c r="K74">
+        <v>0.39065008034001902</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>27</v>
       </c>
@@ -2266,8 +2423,17 @@
       <c r="F75">
         <v>280000</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I75" s="9">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>2.4181191418686E-2</v>
+      </c>
+      <c r="K75">
+        <v>0.39833414043583498</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -2286,8 +2452,17 @@
       <c r="F76">
         <v>82694</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I76" s="9">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>5.2525695195359701E-3</v>
+      </c>
+      <c r="K76">
+        <v>0.21408790156726401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -2306,8 +2481,17 @@
       <c r="F77">
         <v>200000</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I77" s="9">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>9.4100598032879901E-3</v>
+      </c>
+      <c r="K77">
+        <v>0.170621822033898</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -2326,8 +2510,17 @@
       <c r="F78">
         <v>240000</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I78" s="9">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>1.3777144759524499E-3</v>
+      </c>
+      <c r="K78">
+        <v>0.48209039548022597</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>31</v>
       </c>
@@ -2346,8 +2539,17 @@
       <c r="F79">
         <v>50625</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I79" s="9">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>1.3327257204949099E-3</v>
+      </c>
+      <c r="K79">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>32</v>
       </c>
@@ -2366,8 +2568,17 @@
       <c r="F80">
         <v>113564</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I80" s="9">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -2386,8 +2597,17 @@
       <c r="F81">
         <v>6840</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I81" s="9">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>4.9360603929053202E-3</v>
+      </c>
+      <c r="K81">
+        <v>0.56232007136485196</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>34</v>
       </c>
@@ -2406,8 +2626,17 @@
       <c r="F82" s="6">
         <v>112225</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I82" s="9">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>5.88505849332128E-3</v>
+      </c>
+      <c r="K82">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -2426,8 +2655,17 @@
       <c r="F83">
         <v>1749600</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I83" s="9">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>0.48209039548022597</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -2446,8 +2684,17 @@
       <c r="F84">
         <v>1350000</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I84" s="9">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>0.15649365049876601</v>
+      </c>
+      <c r="K84">
+        <v>0.423461016949152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>38</v>
       </c>
@@ -2466,8 +2713,17 @@
       <c r="F85">
         <v>1066485</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I85" s="9">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>0.120754583163302</v>
+      </c>
+      <c r="K85">
+        <v>0.34127483091730998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -2486,8 +2742,17 @@
       <c r="F86">
         <v>699392</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I86" s="9">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>4.0762988121380697E-2</v>
+      </c>
+      <c r="K86">
+        <v>0.48237667174258397</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>40</v>
       </c>
@@ -2506,8 +2771,17 @@
       <c r="F87">
         <v>647000</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I87" s="9">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>5.1053768972684398E-2</v>
+      </c>
+      <c r="K87">
+        <v>0.46479472881355899</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>41</v>
       </c>
@@ -2526,8 +2800,17 @@
       <c r="F88">
         <v>2457600</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I88" s="9">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0.17842434558562301</v>
+      </c>
+      <c r="K88">
+        <v>0.48209039548022597</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -2546,8 +2829,17 @@
       <c r="F89">
         <v>667000</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I89" s="9">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>3.0494966287543699E-2</v>
+      </c>
+      <c r="K89">
+        <v>0.482383542372881</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>43</v>
       </c>
@@ -2566,8 +2858,17 @@
       <c r="F90">
         <v>667000</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I90" s="9">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>3.1358750392328397E-2</v>
+      </c>
+      <c r="K90">
+        <v>0.482383542372881</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>46</v>
       </c>
@@ -2586,8 +2887,17 @@
       <c r="F91">
         <v>360000</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I91" s="9">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>1.2955173733341501E-2</v>
+      </c>
+      <c r="K91">
+        <v>0.77523728813559301</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>47</v>
       </c>
@@ -2606,8 +2916,17 @@
       <c r="F92">
         <v>426756</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I92" s="9">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0.318964454119673</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -2626,8 +2945,17 @@
       <c r="F93">
         <v>53190</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I93" s="9">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>2.5412824759270401E-2</v>
+      </c>
+      <c r="K93">
+        <v>0.537462586315128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>49</v>
       </c>
@@ -2646,8 +2974,17 @@
       <c r="F94">
         <v>53190</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I94" s="9">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>2.48274416588465E-2</v>
+      </c>
+      <c r="K94">
+        <v>0.537462586315128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>50</v>
       </c>
@@ -2666,8 +3003,17 @@
       <c r="F95">
         <v>53190</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I95" s="9">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>3.0499200523351502E-2</v>
+      </c>
+      <c r="K95">
+        <v>0.537462586315128</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>51</v>
       </c>
@@ -2686,8 +3032,17 @@
       <c r="F96">
         <v>53190</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I96" s="9">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>2.8689593995006701E-2</v>
+      </c>
+      <c r="K96">
+        <v>0.537462586315128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>52</v>
       </c>
@@ -2705,6 +3060,15 @@
       </c>
       <c r="F97">
         <v>106800</v>
+      </c>
+      <c r="I97" s="9">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>2.6898512248320901E-2</v>
+      </c>
+      <c r="K97">
+        <v>0.48282326271186399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>